<commit_message>
Added and modified various things, check commit
</commit_message>
<xml_diff>
--- a/analysis/xlsx/researcher_network_a_analysis.xlsx
+++ b/analysis/xlsx/researcher_network_a_analysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="13200" windowHeight="4440"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="13200" windowHeight="4440" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Glossary" sheetId="11" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="48">
   <si>
     <t>Nodes</t>
   </si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t>C1-8</t>
+  </si>
+  <si>
+    <t>Latex format</t>
   </si>
 </sst>
 </file>
@@ -208,7 +211,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -438,11 +441,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -558,6 +572,10 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -584,6 +602,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -881,7 +905,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -929,26 +953,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="28.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" customWidth="1"/>
+    <col min="8" max="8" width="55.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6">
+    <row r="1" spans="2:9">
       <c r="F1" s="18"/>
-    </row>
-    <row r="2" spans="2:6" ht="15.75" thickBot="1">
+      <c r="I1" s="18"/>
+    </row>
+    <row r="2" spans="2:9" ht="15.75" thickBot="1">
       <c r="F2" s="18"/>
-    </row>
-    <row r="3" spans="2:6" ht="15.75" thickBot="1">
+      <c r="I2" s="18"/>
+    </row>
+    <row r="3" spans="2:9" ht="15.75" thickBot="1">
       <c r="B3" s="42" t="s">
         <v>40</v>
       </c>
@@ -962,8 +988,12 @@
         <v>25</v>
       </c>
       <c r="F3" s="18"/>
-    </row>
-    <row r="4" spans="2:6">
+      <c r="H3" s="57" t="s">
+        <v>47</v>
+      </c>
+      <c r="I3" s="18"/>
+    </row>
+    <row r="4" spans="2:9">
       <c r="B4" s="11" t="s">
         <v>0</v>
       </c>
@@ -977,8 +1007,13 @@
         <v>655</v>
       </c>
       <c r="F4" s="18"/>
-    </row>
-    <row r="5" spans="2:6">
+      <c r="H4" s="56" t="str">
+        <f>"\textbf{"&amp;B4&amp;"}"&amp;" &amp; "&amp;"{"&amp;C4&amp;"}"&amp;" &amp; "&amp;"{"&amp;E4&amp;"}"&amp;"\\"</f>
+        <v>\textbf{Nodes} &amp; {655} &amp; {655}\\</v>
+      </c>
+      <c r="I4" s="18"/>
+    </row>
+    <row r="5" spans="2:9">
       <c r="B5" s="11" t="s">
         <v>1</v>
       </c>
@@ -992,8 +1027,13 @@
         <v>4548</v>
       </c>
       <c r="F5" s="18"/>
-    </row>
-    <row r="6" spans="2:6">
+      <c r="H5" s="45" t="str">
+        <f t="shared" ref="H5:H22" si="0">"\textbf{"&amp;B5&amp;"}"&amp;" &amp; "&amp;"{"&amp;C5&amp;"}"&amp;" &amp; "&amp;"{"&amp;E5&amp;"}"&amp;"\\"</f>
+        <v>\textbf{Edges} &amp; {4548} &amp; {4548}\\</v>
+      </c>
+      <c r="I5" s="18"/>
+    </row>
+    <row r="6" spans="2:9">
       <c r="B6" s="11" t="s">
         <v>2</v>
       </c>
@@ -1007,8 +1047,13 @@
         <v>19</v>
       </c>
       <c r="F6" s="18"/>
-    </row>
-    <row r="7" spans="2:6">
+      <c r="H6" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v>\textbf{Type} &amp; {Undirected} &amp; {Undirected}\\</v>
+      </c>
+      <c r="I6" s="18"/>
+    </row>
+    <row r="7" spans="2:9">
       <c r="B7" s="11" t="s">
         <v>3</v>
       </c>
@@ -1022,8 +1067,13 @@
         <v>21</v>
       </c>
       <c r="F7" s="18"/>
-    </row>
-    <row r="8" spans="2:6">
+      <c r="H7" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v>\textbf{Weighted} &amp; {No} &amp; {Yes}\\</v>
+      </c>
+      <c r="I7" s="18"/>
+    </row>
+    <row r="8" spans="2:9">
       <c r="B8" s="11" t="s">
         <v>4</v>
       </c>
@@ -1037,8 +1087,13 @@
         <v>20</v>
       </c>
       <c r="F8" s="18"/>
-    </row>
-    <row r="9" spans="2:6">
+      <c r="H8" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v>\textbf{Connected} &amp; {No} &amp; {No}\\</v>
+      </c>
+      <c r="I8" s="18"/>
+    </row>
+    <row r="9" spans="2:9">
       <c r="B9" s="11" t="s">
         <v>5</v>
       </c>
@@ -1052,8 +1107,13 @@
         <v>13.887</v>
       </c>
       <c r="F9" s="18"/>
-    </row>
-    <row r="10" spans="2:6">
+      <c r="H9" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v>\textbf{Average Degree} &amp; {13.887} &amp; {13.887}\\</v>
+      </c>
+      <c r="I9" s="18"/>
+    </row>
+    <row r="10" spans="2:9">
       <c r="B10" s="11" t="s">
         <v>6</v>
       </c>
@@ -1067,8 +1127,13 @@
         <v>27.257999999999999</v>
       </c>
       <c r="F10" s="18"/>
-    </row>
-    <row r="11" spans="2:6">
+      <c r="H10" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v>\textbf{Average Weighted Degree} &amp; {-} &amp; {27.258}\\</v>
+      </c>
+      <c r="I10" s="18"/>
+    </row>
+    <row r="11" spans="2:9">
       <c r="B11" s="11" t="s">
         <v>7</v>
       </c>
@@ -1082,8 +1147,13 @@
         <v>15</v>
       </c>
       <c r="F11" s="18"/>
-    </row>
-    <row r="12" spans="2:6">
+      <c r="H11" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v>\textbf{Diameter} &amp; {12} &amp; {15}\\</v>
+      </c>
+      <c r="I11" s="18"/>
+    </row>
+    <row r="12" spans="2:9">
       <c r="B12" s="11" t="s">
         <v>8</v>
       </c>
@@ -1097,8 +1167,13 @@
         <v>1</v>
       </c>
       <c r="F12" s="18"/>
-    </row>
-    <row r="13" spans="2:6">
+      <c r="H12" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v>\textbf{Radius} &amp; {1} &amp; {1}\\</v>
+      </c>
+      <c r="I12" s="18"/>
+    </row>
+    <row r="13" spans="2:9">
       <c r="B13" s="11" t="s">
         <v>9</v>
       </c>
@@ -1112,8 +1187,13 @@
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="F13" s="18"/>
-    </row>
-    <row r="14" spans="2:6">
+      <c r="H13" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v>\textbf{Density} &amp; {0.021} &amp; {0.021}\\</v>
+      </c>
+      <c r="I13" s="18"/>
+    </row>
+    <row r="14" spans="2:9">
       <c r="B14" s="11" t="s">
         <v>10</v>
       </c>
@@ -1127,8 +1207,13 @@
         <v>0.73799999999999999</v>
       </c>
       <c r="F14" s="18"/>
-    </row>
-    <row r="15" spans="2:6">
+      <c r="H14" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v>\textbf{Modularity} &amp; {0.745} &amp; {0.738}\\</v>
+      </c>
+      <c r="I14" s="18"/>
+    </row>
+    <row r="15" spans="2:9">
       <c r="B15" s="11" t="s">
         <v>11</v>
       </c>
@@ -1142,8 +1227,13 @@
         <v>49</v>
       </c>
       <c r="F15" s="18"/>
-    </row>
-    <row r="16" spans="2:6">
+      <c r="H15" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v>\textbf{Communities} &amp; {46} &amp; {49}\\</v>
+      </c>
+      <c r="I15" s="18"/>
+    </row>
+    <row r="16" spans="2:9">
       <c r="B16" s="11" t="s">
         <v>12</v>
       </c>
@@ -1157,8 +1247,13 @@
         <v>39</v>
       </c>
       <c r="F16" s="18"/>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="H16" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v>\textbf{Weak Components} &amp; {39} &amp; {39}\\</v>
+      </c>
+      <c r="I16" s="18"/>
+    </row>
+    <row r="17" spans="1:9">
       <c r="B17" s="11" t="s">
         <v>13</v>
       </c>
@@ -1172,8 +1267,13 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F17" s="18"/>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="H17" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v>\textbf{Node Closeness} &amp; {0.005} &amp; {0.005}\\</v>
+      </c>
+      <c r="I17" s="18"/>
+    </row>
+    <row r="18" spans="1:9">
       <c r="B18" s="11" t="s">
         <v>14</v>
       </c>
@@ -1187,8 +1287,13 @@
         <v>703.13800000000003</v>
       </c>
       <c r="F18" s="18"/>
-    </row>
-    <row r="19" spans="1:6" ht="15.75" thickBot="1">
+      <c r="H18" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v>\textbf{Node Betweenness} &amp; {594.569} &amp; {703.138}\\</v>
+      </c>
+      <c r="I18" s="18"/>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" thickBot="1">
       <c r="B19" s="12" t="s">
         <v>15</v>
       </c>
@@ -1202,8 +1307,13 @@
         <v>127.386</v>
       </c>
       <c r="F19" s="18"/>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="H19" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v>\textbf{Edge Betweenness} &amp; {111.75} &amp; {127.386}\\</v>
+      </c>
+      <c r="I19" s="18"/>
+    </row>
+    <row r="20" spans="1:9">
       <c r="B20" s="40" t="s">
         <v>16</v>
       </c>
@@ -1217,8 +1327,13 @@
         <v>0.82499999999999996</v>
       </c>
       <c r="F20" s="18"/>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" thickBot="1">
+      <c r="H20" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v>\textbf{Average Clustering Coefficient} &amp; {0.825} &amp; {0.825}\\</v>
+      </c>
+      <c r="I20" s="18"/>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" thickBot="1">
       <c r="B21" s="12" t="s">
         <v>17</v>
       </c>
@@ -1232,8 +1347,13 @@
         <v>7.8E-2</v>
       </c>
       <c r="F21" s="18"/>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="H21" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v>\textbf{Eigenvector Centrality} &amp; {0.092} &amp; {0.078}\\</v>
+      </c>
+      <c r="I21" s="18"/>
+    </row>
+    <row r="22" spans="1:9">
       <c r="B22" s="40" t="s">
         <v>18</v>
       </c>
@@ -1247,21 +1367,30 @@
         <v>4.2779999999999996</v>
       </c>
       <c r="F22" s="18"/>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="H22" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v>\textbf{Average Path Length} &amp; {4.278} &amp; {4.278}\\</v>
+      </c>
+      <c r="I22" s="18"/>
+    </row>
+    <row r="23" spans="1:9">
       <c r="B23" s="22"/>
       <c r="C23" s="27"/>
       <c r="D23" s="27"/>
       <c r="E23" s="28"/>
       <c r="F23" s="18"/>
-    </row>
-    <row r="24" spans="1:6" ht="15.75" thickBot="1">
+      <c r="I23" s="18"/>
+    </row>
+    <row r="24" spans="1:9" ht="15.75" thickBot="1">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="F24" s="19"/>
+      <c r="G24" s="46"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1271,10 +1400,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:L39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1282,33 +1411,40 @@
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="11" max="11" width="57.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:12">
       <c r="I1" s="18"/>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1">
+      <c r="L1" s="18"/>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" thickBot="1">
       <c r="I2" s="18"/>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1">
+      <c r="L2" s="18"/>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" thickBot="1">
       <c r="B3" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46" t="s">
+      <c r="D3" s="48"/>
+      <c r="E3" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46" t="s">
+      <c r="F3" s="48"/>
+      <c r="G3" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="46"/>
+      <c r="H3" s="48"/>
       <c r="I3" s="18"/>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="K3" s="57" t="s">
+        <v>47</v>
+      </c>
+      <c r="L3" s="18"/>
+    </row>
+    <row r="4" spans="1:12">
       <c r="B4" s="40" t="s">
         <v>26</v>
       </c>
@@ -1331,8 +1467,13 @@
         <v>0.71</v>
       </c>
       <c r="I4" s="18"/>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="K4" s="56" t="str">
+        <f>"\textbf"&amp;"{"&amp;B4&amp;"}"&amp;" &amp; "&amp;"{"&amp;C4&amp;"}"&amp;" &amp; "&amp;"{"&amp;D4&amp;"}"&amp;" &amp; "&amp;"{"&amp;G4&amp;"}"&amp;" &amp; "&amp;"{"&amp;H4&amp;"}"&amp;"\\"</f>
+        <v>\textbf{Infomap} &amp; {78} &amp; {0.716} &amp; {84} &amp; {0.71}\\</v>
+      </c>
+      <c r="L4" s="18"/>
+    </row>
+    <row r="5" spans="1:12">
       <c r="B5" s="11" t="s">
         <v>27</v>
       </c>
@@ -1355,8 +1496,13 @@
         <v>22</v>
       </c>
       <c r="I5" s="18"/>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="K5" s="45" t="str">
+        <f t="shared" ref="K5:K11" si="0">"\textbf"&amp;"{"&amp;B5&amp;"}"&amp;" &amp; "&amp;"{"&amp;C5&amp;"}"&amp;" &amp; "&amp;"{"&amp;D5&amp;"}"&amp;" &amp; "&amp;"{"&amp;G5&amp;"}"&amp;" &amp; "&amp;"{"&amp;H5&amp;"}"&amp;"\\"</f>
+        <v>\textbf{Spinglass} &amp; {-} &amp; {-} &amp; {-} &amp; {-}\\</v>
+      </c>
+      <c r="L5" s="18"/>
+    </row>
+    <row r="6" spans="1:12">
       <c r="B6" s="11" t="s">
         <v>28</v>
       </c>
@@ -1379,8 +1525,13 @@
         <v>0.73799999999999999</v>
       </c>
       <c r="I6" s="18"/>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="K6" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v>\textbf{Louvain} &amp; {46} &amp; {0.745} &amp; {49} &amp; {0.738}\\</v>
+      </c>
+      <c r="L6" s="18"/>
+    </row>
+    <row r="7" spans="1:12">
       <c r="B7" s="11" t="s">
         <v>29</v>
       </c>
@@ -1403,8 +1554,13 @@
         <v>0.72</v>
       </c>
       <c r="I7" s="18"/>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="K7" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v>\textbf{Label Propagation} &amp; {69} &amp; {0.72} &amp; {71} &amp; {0.72}\\</v>
+      </c>
+      <c r="L7" s="18"/>
+    </row>
+    <row r="8" spans="1:12">
       <c r="B8" s="11" t="s">
         <v>30</v>
       </c>
@@ -1427,8 +1583,13 @@
         <v>0.68200000000000005</v>
       </c>
       <c r="I8" s="18"/>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="K8" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v>\textbf{Leading Eigenvector} &amp; {41} &amp; {0.721} &amp; {45} &amp; {0.682}\\</v>
+      </c>
+      <c r="L8" s="18"/>
+    </row>
+    <row r="9" spans="1:12">
       <c r="B9" s="11" t="s">
         <v>31</v>
       </c>
@@ -1451,8 +1612,13 @@
         <v>0.72</v>
       </c>
       <c r="I9" s="18"/>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="K9" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v>\textbf{Walktrap} &amp; {61} &amp; {0.734} &amp; {81} &amp; {0.72}\\</v>
+      </c>
+      <c r="L9" s="18"/>
+    </row>
+    <row r="10" spans="1:12">
       <c r="B10" s="11" t="s">
         <v>32</v>
       </c>
@@ -1475,8 +1641,13 @@
         <v>0.73399999999999999</v>
       </c>
       <c r="I10" s="18"/>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="K10" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v>\textbf{Fast Greedy} &amp; {49} &amp; {0.741} &amp; {48} &amp; {0.734}\\</v>
+      </c>
+      <c r="L10" s="18"/>
+    </row>
+    <row r="11" spans="1:12">
       <c r="B11" s="11" t="s">
         <v>15</v>
       </c>
@@ -1499,8 +1670,13 @@
         <v>22</v>
       </c>
       <c r="I11" s="18"/>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="K11" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v>\textbf{Edge Betweenness} &amp; {-} &amp; {-} &amp; {-} &amp; {-}\\</v>
+      </c>
+      <c r="L11" s="18"/>
+    </row>
+    <row r="12" spans="1:12">
       <c r="B12" s="22"/>
       <c r="C12" s="26"/>
       <c r="D12" s="27"/>
@@ -1509,8 +1685,9 @@
       <c r="G12" s="26"/>
       <c r="H12" s="27"/>
       <c r="I12" s="18"/>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" thickBot="1">
+      <c r="L12" s="18"/>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" thickBot="1">
       <c r="A13" s="8"/>
       <c r="B13" s="29"/>
       <c r="C13" s="30"/>
@@ -1520,8 +1697,11 @@
       <c r="G13" s="30"/>
       <c r="H13" s="31"/>
       <c r="I13" s="19"/>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="J13" s="46"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="19"/>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" s="20"/>
       <c r="B14" s="22"/>
       <c r="C14" s="26"/>
@@ -1560,48 +1740,52 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:B14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="71.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14">
+    <row r="1" spans="2:15">
       <c r="L1" s="18"/>
       <c r="M1" s="20"/>
       <c r="N1" s="20"/>
-    </row>
-    <row r="2" spans="2:14" ht="15.75" thickBot="1">
+      <c r="O1" s="18"/>
+    </row>
+    <row r="2" spans="2:15" ht="15.75" thickBot="1">
       <c r="L2" s="18"/>
       <c r="M2" s="20"/>
       <c r="N2" s="20"/>
-    </row>
-    <row r="3" spans="2:14" ht="15.75" thickBot="1">
+      <c r="O2" s="18"/>
+    </row>
+    <row r="3" spans="2:15" ht="15.75" thickBot="1">
       <c r="B3" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46" t="s">
+      <c r="D3" s="48"/>
+      <c r="E3" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46" t="s">
+      <c r="F3" s="48"/>
+      <c r="G3" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="46"/>
+      <c r="H3" s="48"/>
       <c r="I3" s="20"/>
       <c r="J3" s="20"/>
       <c r="K3" s="20"/>
       <c r="L3" s="18"/>
-    </row>
-    <row r="4" spans="2:14">
+      <c r="O3" s="18"/>
+    </row>
+    <row r="4" spans="2:15">
       <c r="B4" s="40" t="s">
         <v>27</v>
       </c>
@@ -1627,8 +1811,9 @@
       <c r="J4" s="20"/>
       <c r="K4" s="20"/>
       <c r="L4" s="18"/>
-    </row>
-    <row r="5" spans="2:14">
+      <c r="O4" s="18"/>
+    </row>
+    <row r="5" spans="2:15">
       <c r="B5" s="11" t="s">
         <v>28</v>
       </c>
@@ -1654,8 +1839,9 @@
       <c r="J5" s="20"/>
       <c r="K5" s="20"/>
       <c r="L5" s="18"/>
-    </row>
-    <row r="6" spans="2:14">
+      <c r="O5" s="18"/>
+    </row>
+    <row r="6" spans="2:15">
       <c r="B6" s="11" t="s">
         <v>32</v>
       </c>
@@ -1681,17 +1867,19 @@
       <c r="J6" s="20"/>
       <c r="K6" s="20"/>
       <c r="L6" s="18"/>
-    </row>
-    <row r="7" spans="2:14" ht="15.75" thickBot="1">
+      <c r="O6" s="18"/>
+    </row>
+    <row r="7" spans="2:15" ht="15.75" thickBot="1">
       <c r="L7" s="18"/>
       <c r="M7" s="20"/>
       <c r="N7" s="20"/>
-    </row>
-    <row r="8" spans="2:14" ht="15.75" thickBot="1">
-      <c r="B8" s="52" t="s">
+      <c r="O7" s="18"/>
+    </row>
+    <row r="8" spans="2:15" ht="15.75" thickBot="1">
+      <c r="B8" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="53"/>
+      <c r="C8" s="55"/>
       <c r="D8" s="41" t="s">
         <v>33</v>
       </c>
@@ -1718,10 +1906,13 @@
       </c>
       <c r="L8" s="18"/>
       <c r="M8" s="20"/>
-      <c r="N8" s="20"/>
-    </row>
-    <row r="9" spans="2:14">
-      <c r="B9" s="50" t="s">
+      <c r="N8" s="57" t="s">
+        <v>47</v>
+      </c>
+      <c r="O8" s="18"/>
+    </row>
+    <row r="9" spans="2:15">
+      <c r="B9" s="52" t="s">
         <v>23</v>
       </c>
       <c r="C9" s="40" t="s">
@@ -1753,10 +1944,14 @@
       </c>
       <c r="L9" s="18"/>
       <c r="M9" s="20"/>
-      <c r="N9" s="20"/>
-    </row>
-    <row r="10" spans="2:14">
-      <c r="B10" s="50"/>
+      <c r="N9" s="56" t="str">
+        <f>"&amp; "&amp;"\textbf{"&amp;C9&amp;"}"&amp;" &amp; "&amp;"{"&amp;D9&amp;"}"&amp;" &amp; "&amp;"{"&amp;E9&amp;"}"&amp;" &amp; "&amp;"{"&amp;F9&amp;"}"&amp;" &amp; "&amp;"{"&amp;G9&amp;"}"&amp;" &amp; "&amp;"{"&amp;H9&amp;"}"&amp;" &amp; "&amp;"{"&amp;I9&amp;"}"&amp;" &amp; "&amp;"{"&amp;J9&amp;"}"&amp;" &amp; "&amp;"{"&amp;K9&amp;"}"&amp;"\\"</f>
+        <v>&amp; \textbf{Spinglass} &amp; {-} &amp; {-} &amp; {-} &amp; {-} &amp; {-} &amp; {-} &amp; {-} &amp; {-}\\</v>
+      </c>
+      <c r="O9" s="18"/>
+    </row>
+    <row r="10" spans="2:15">
+      <c r="B10" s="52"/>
       <c r="C10" s="11" t="s">
         <v>28</v>
       </c>
@@ -1786,10 +1981,14 @@
       </c>
       <c r="L10" s="18"/>
       <c r="M10" s="20"/>
-      <c r="N10" s="20"/>
-    </row>
-    <row r="11" spans="2:14" ht="15.75" thickBot="1">
-      <c r="B11" s="51"/>
+      <c r="N10" s="45" t="str">
+        <f t="shared" ref="N10:N17" si="0">"&amp; "&amp;"\textbf{"&amp;C10&amp;"}"&amp;" &amp; "&amp;"{"&amp;D10&amp;"}"&amp;" &amp; "&amp;"{"&amp;E10&amp;"}"&amp;" &amp; "&amp;"{"&amp;F10&amp;"}"&amp;" &amp; "&amp;"{"&amp;G10&amp;"}"&amp;" &amp; "&amp;"{"&amp;H10&amp;"}"&amp;" &amp; "&amp;"{"&amp;I10&amp;"}"&amp;" &amp; "&amp;"{"&amp;J10&amp;"}"&amp;" &amp; "&amp;"{"&amp;K10&amp;"}"&amp;"\\"</f>
+        <v>&amp; \textbf{Louvain} &amp; {60} &amp; {118} &amp; {73} &amp; {132} &amp; {87} &amp; {46} &amp; {-} &amp; {-}\\</v>
+      </c>
+      <c r="O10" s="18"/>
+    </row>
+    <row r="11" spans="2:15" ht="15.75" thickBot="1">
+      <c r="B11" s="53"/>
       <c r="C11" s="12" t="s">
         <v>32</v>
       </c>
@@ -1819,10 +2018,14 @@
       </c>
       <c r="L11" s="18"/>
       <c r="M11" s="20"/>
-      <c r="N11" s="20"/>
-    </row>
-    <row r="12" spans="2:14">
-      <c r="B12" s="49" t="s">
+      <c r="N11" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v>&amp; \textbf{Fast Greedy} &amp; {161} &amp; {60} &amp; {73} &amp; {145} &amp; {24} &amp; {36} &amp; {-} &amp; {-}\\</v>
+      </c>
+      <c r="O11" s="18"/>
+    </row>
+    <row r="12" spans="2:15">
+      <c r="B12" s="51" t="s">
         <v>24</v>
       </c>
       <c r="C12" s="13" t="s">
@@ -1854,10 +2057,14 @@
       </c>
       <c r="L12" s="18"/>
       <c r="M12" s="20"/>
-      <c r="N12" s="20"/>
-    </row>
-    <row r="13" spans="2:14">
-      <c r="B13" s="50"/>
+      <c r="N12" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v>&amp; \textbf{Spinglass} &amp; {-} &amp; {-} &amp; {-} &amp; {-} &amp; {-} &amp; {-} &amp; {-} &amp; {-}\\</v>
+      </c>
+      <c r="O12" s="18"/>
+    </row>
+    <row r="13" spans="2:15">
+      <c r="B13" s="52"/>
       <c r="C13" s="11" t="s">
         <v>28</v>
       </c>
@@ -1887,10 +2094,14 @@
       </c>
       <c r="L13" s="18"/>
       <c r="M13" s="20"/>
-      <c r="N13" s="20"/>
-    </row>
-    <row r="14" spans="2:14" ht="15.75" thickBot="1">
-      <c r="B14" s="51"/>
+      <c r="N13" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v>&amp; \textbf{Louvain} &amp; {60} &amp; {64} &amp; {24} &amp; {111} &amp; {73} &amp; {22} &amp; {116} &amp; {46}\\</v>
+      </c>
+      <c r="O13" s="18"/>
+    </row>
+    <row r="14" spans="2:15" ht="15.75" thickBot="1">
+      <c r="B14" s="53"/>
       <c r="C14" s="12" t="s">
         <v>32</v>
       </c>
@@ -1920,10 +2131,14 @@
       </c>
       <c r="L14" s="18"/>
       <c r="M14" s="20"/>
-      <c r="N14" s="20"/>
-    </row>
-    <row r="15" spans="2:14">
-      <c r="B15" s="47" t="s">
+      <c r="N14" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v>&amp; \textbf{Fast Greedy} &amp; {161} &amp; {60} &amp; {73} &amp; {145} &amp; {24} &amp; {36} &amp; {-} &amp; {-}\\</v>
+      </c>
+      <c r="O14" s="18"/>
+    </row>
+    <row r="15" spans="2:15">
+      <c r="B15" s="49" t="s">
         <v>25</v>
       </c>
       <c r="C15" s="13" t="s">
@@ -1955,10 +2170,14 @@
       </c>
       <c r="L15" s="18"/>
       <c r="M15" s="20"/>
-      <c r="N15" s="20"/>
-    </row>
-    <row r="16" spans="2:14">
-      <c r="B16" s="48"/>
+      <c r="N15" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v>&amp; \textbf{Spinglass} &amp; {-} &amp; {-} &amp; {-} &amp; {-} &amp; {-} &amp; {-} &amp; {-} &amp; {-}\\</v>
+      </c>
+      <c r="O15" s="18"/>
+    </row>
+    <row r="16" spans="2:15">
+      <c r="B16" s="50"/>
       <c r="C16" s="11" t="s">
         <v>28</v>
       </c>
@@ -1988,10 +2207,14 @@
       </c>
       <c r="L16" s="18"/>
       <c r="M16" s="20"/>
-      <c r="N16" s="20"/>
+      <c r="N16" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v>&amp; \textbf{Louvain} &amp; {60} &amp; {120} &amp; {30} &amp; {24} &amp; {43} &amp; {48} &amp; {126} &amp; {46}\\</v>
+      </c>
+      <c r="O16" s="18"/>
     </row>
     <row r="17" spans="1:15">
-      <c r="B17" s="48"/>
+      <c r="B17" s="50"/>
       <c r="C17" s="11" t="s">
         <v>32</v>
       </c>
@@ -2021,7 +2244,11 @@
       </c>
       <c r="L17" s="18"/>
       <c r="M17" s="20"/>
-      <c r="N17" s="20"/>
+      <c r="N17" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v>&amp; \textbf{Fast Greedy} &amp; {54} &amp; {60} &amp; {73} &amp; {126} &amp; {46} &amp; {133} &amp; {24} &amp; {-}\\</v>
+      </c>
+      <c r="O17" s="18"/>
     </row>
     <row r="18" spans="1:15">
       <c r="B18" s="21"/>
@@ -2037,6 +2264,7 @@
       <c r="L18" s="18"/>
       <c r="M18" s="20"/>
       <c r="N18" s="20"/>
+      <c r="O18" s="18"/>
     </row>
     <row r="19" spans="1:15" s="20" customFormat="1" ht="15.75" thickBot="1">
       <c r="A19" s="8"/>
@@ -2051,6 +2279,9 @@
       <c r="J19" s="8"/>
       <c r="K19" s="8"/>
       <c r="L19" s="19"/>
+      <c r="M19" s="46"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="19"/>
     </row>
     <row r="20" spans="1:15">
       <c r="M20" s="20"/>

</xml_diff>